<commit_message>
corrected metadata column male
</commit_message>
<xml_diff>
--- a/Salary metadata.xlsx
+++ b/Salary metadata.xlsx
@@ -80,9 +80,6 @@
     <t>Position (1 = Junior Employee, 2 = Manager, 3 = Executive)</t>
   </si>
   <si>
-    <t>0 = yes, 1 = no</t>
-  </si>
-  <si>
     <t>Years absent from work (e.g. due to illness / child rearing / personal reasons)</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>Field of work (1 = Engineering, 2 = Finance, 3 = Human Resources, 4 = Marketing)</t>
+  </si>
+  <si>
+    <t>0 = no, 1 = yes</t>
   </si>
 </sst>
 </file>
@@ -462,7 +462,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -473,13 +473,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -487,7 +487,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -498,7 +498,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -509,7 +509,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -520,7 +520,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
@@ -531,7 +531,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
@@ -542,7 +542,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
@@ -553,7 +553,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
@@ -564,7 +564,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
@@ -575,21 +575,21 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
         <v>26</v>
-      </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -597,10 +597,10 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>